<commit_message>
Septima Actualizacion de Proyecto + Calendario de Responsabilidades
</commit_message>
<xml_diff>
--- a/Calendario-Responsabilidades.xlsx
+++ b/Calendario-Responsabilidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMETH\IdeaProjects\Proyecto-Dorikam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1567247F-A4EB-4BE7-B947-28764E773295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C64CDB-2303-4FE1-B920-A26CB1F20B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00253EC3-853E-4A73-9C54-93DBFD01F7E4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>AdministradorController</t>
   </si>
@@ -73,13 +73,16 @@
   </si>
   <si>
     <t>EliminarProductoController</t>
+  </si>
+  <si>
+    <t>"25/03/2024" al "31/03/2024"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,14 +114,6 @@
       <name val="Adobe Fan Heiti Std B"/>
       <family val="2"/>
       <charset val="128"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -168,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -194,14 +189,35 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -539,7 +555,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,6 +563,7 @@
     <col min="1" max="1" width="33.88671875" customWidth="1"/>
     <col min="3" max="3" width="29.6640625" customWidth="1"/>
     <col min="4" max="4" width="29.88671875" customWidth="1"/>
+    <col min="5" max="5" width="30.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -562,6 +579,9 @@
       <c r="D1" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -571,9 +591,12 @@
         <v>90</v>
       </c>
       <c r="C2" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7">
         <v>0</v>
       </c>
     </row>
@@ -590,6 +613,9 @@
       <c r="D3" s="8">
         <v>0</v>
       </c>
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -599,9 +625,12 @@
         <v>0</v>
       </c>
       <c r="C4" s="8">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
         <v>0</v>
       </c>
     </row>
@@ -618,6 +647,9 @@
       <c r="D5" s="8">
         <v>0</v>
       </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -632,7 +664,9 @@
       <c r="D6" s="8">
         <v>0</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -647,18 +681,24 @@
       <c r="D7" s="8">
         <v>0</v>
       </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="8">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C8" s="8">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
         <v>0</v>
       </c>
     </row>
@@ -667,12 +707,15 @@
         <v>4</v>
       </c>
       <c r="B9" s="8">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C9" s="8">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8">
         <v>0</v>
       </c>
     </row>
@@ -681,12 +724,15 @@
         <v>5</v>
       </c>
       <c r="B10" s="8">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C10" s="8">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8">
         <v>0</v>
       </c>
     </row>
@@ -695,12 +741,15 @@
         <v>6</v>
       </c>
       <c r="B11" s="8">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C11" s="8">
         <v>88</v>
       </c>
       <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8">
         <v>0</v>
       </c>
     </row>
@@ -712,9 +761,12 @@
         <v>0</v>
       </c>
       <c r="C12" s="8">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8">
         <v>0</v>
       </c>
     </row>
@@ -726,15 +778,18 @@
         <v>0</v>
       </c>
       <c r="C13" s="8">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B13">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -746,20 +801,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:D13">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
       <formula>0</formula>
       <formula>40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="between">
       <formula>50</formula>
       <formula>70</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C13">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
@@ -771,8 +838,22 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D13">
-    <cfRule type="colorScale" priority="13">
+  <conditionalFormatting sqref="E2:E13">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+      <formula>80</formula>
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>0</formula>
+      <formula>40</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
+      <formula>50</formula>
+      <formula>70</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E13">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>

</xml_diff>

<commit_message>
Logica para agregar y eliminar imagenes de catalago de ofertas
</commit_message>
<xml_diff>
--- a/Calendario-Responsabilidades.xlsx
+++ b/Calendario-Responsabilidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMETH\IdeaProjects\Proyecto-Dorikam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C64CDB-2303-4FE1-B920-A26CB1F20B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19410A2B-11FF-4419-A014-19BFFE36D8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00253EC3-853E-4A73-9C54-93DBFD01F7E4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>AdministradorController</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>"25/03/2024" al "31/03/2024"</t>
+  </si>
+  <si>
+    <t>App</t>
   </si>
 </sst>
 </file>
@@ -193,7 +196,79 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -552,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2790D138-02F1-46FC-AFAF-C1A947E3BEF4}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -787,9 +862,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="14" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="8">
+        <v>70</v>
+      </c>
+      <c r="C14" s="8">
+        <v>90</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B13">
-    <cfRule type="colorScale" priority="26">
+  <conditionalFormatting sqref="B2:B14">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -800,22 +892,22 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:D13">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
+  <conditionalFormatting sqref="B2:E13">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="between">
       <formula>0</formula>
       <formula>40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="between">
       <formula>50</formula>
       <formula>70</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -827,7 +919,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D13">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -839,20 +931,84 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E13">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="between">
       <formula>0</formula>
       <formula>40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="between">
       <formula>50</formula>
       <formula>70</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E13">
+  <conditionalFormatting sqref="C14">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
+      <formula>80</formula>
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="between">
+      <formula>0</formula>
+      <formula>40</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="between">
+      <formula>50</formula>
+      <formula>70</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
+      <formula>80</formula>
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
+      <formula>0</formula>
+      <formula>40</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="between">
+      <formula>50</formula>
+      <formula>70</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
@@ -864,6 +1020,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+      <formula>80</formula>
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>0</formula>
+      <formula>40</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
+      <formula>50</formula>
+      <formula>70</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Interfaz de reportes terminada (100%)
</commit_message>
<xml_diff>
--- a/Calendario-Responsabilidades.xlsx
+++ b/Calendario-Responsabilidades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMETH\IdeaProjects\Proyecto-Dorikam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rumba Hospitality\Documents\ProyectosJavaFX\Proyecto-Dorikam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19410A2B-11FF-4419-A014-19BFFE36D8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA516B87-AC13-46F7-8099-85B92262AF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00253EC3-853E-4A73-9C54-93DBFD01F7E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00253EC3-853E-4A73-9C54-93DBFD01F7E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>AdministradorController</t>
   </si>
@@ -79,13 +79,16 @@
   </si>
   <si>
     <t>App</t>
+  </si>
+  <si>
+    <t>VerReportesController</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -627,21 +630,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2790D138-02F1-46FC-AFAF-C1A947E3BEF4}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="27.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="27.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.88671875" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" customWidth="1"/>
-    <col min="4" max="4" width="29.88671875" customWidth="1"/>
-    <col min="5" max="5" width="30.21875" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="25.15" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -658,7 +661,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -675,7 +678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -692,7 +695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -709,7 +712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -726,7 +729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -743,7 +746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -760,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -777,7 +780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -794,7 +797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -811,7 +814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -828,7 +831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="25.15" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -845,7 +848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="25.15" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -856,13 +859,13 @@
         <v>85</v>
       </c>
       <c r="D13" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E13" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="25.15" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -879,9 +882,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="15" spans="1:5" ht="24" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8">
+        <v>85</v>
+      </c>
+      <c r="D15" s="8">
+        <v>100</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B14">
-    <cfRule type="colorScale" priority="41">
+  <conditionalFormatting sqref="B2:B15">
+    <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -892,22 +912,22 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E13">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="between">
+  <conditionalFormatting sqref="B2:E14">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="between">
       <formula>0</formula>
       <formula>40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="between">
       <formula>50</formula>
       <formula>70</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="colorScale" priority="36">
+    <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -918,8 +938,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D13">
-    <cfRule type="colorScale" priority="32">
+  <conditionalFormatting sqref="C14">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -930,8 +950,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E13">
-    <cfRule type="colorScale" priority="19">
+  <conditionalFormatting sqref="D2:D13">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -942,22 +962,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="between">
-      <formula>80</formula>
-      <formula>100</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="between">
-      <formula>0</formula>
-      <formula>40</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="between">
-      <formula>50</formula>
-      <formula>70</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="D14">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -968,22 +974,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
-      <formula>80</formula>
-      <formula>100</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="between">
-      <formula>0</formula>
-      <formula>40</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="between">
-      <formula>50</formula>
-      <formula>70</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="E2:E13">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -994,22 +986,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
-      <formula>80</formula>
-      <formula>100</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
-      <formula>0</formula>
-      <formula>40</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="between">
-      <formula>50</formula>
-      <formula>70</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="E14:E15">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -1020,7 +998,73 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
+  <conditionalFormatting sqref="B15">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="between">
+      <formula>80</formula>
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="between">
+      <formula>0</formula>
+      <formula>40</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="between">
+      <formula>50</formula>
+      <formula>70</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="between">
+      <formula>80</formula>
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="between">
+      <formula>0</formula>
+      <formula>40</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="between">
+      <formula>50</formula>
+      <formula>70</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="between">
+      <formula>80</formula>
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
+      <formula>0</formula>
+      <formula>40</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="between">
+      <formula>50</formula>
+      <formula>70</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>80</formula>
       <formula>100</formula>

</xml_diff>

<commit_message>
Metodos para usar tecla enter en el pryecto
</commit_message>
<xml_diff>
--- a/Calendario-Responsabilidades.xlsx
+++ b/Calendario-Responsabilidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMETH\IdeaProjects\Proyecto-Dorikam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19410A2B-11FF-4419-A014-19BFFE36D8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FB41E6-6D8A-4C2B-B7BA-FF2B7DF64571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00253EC3-853E-4A73-9C54-93DBFD01F7E4}"/>
   </bookViews>
@@ -196,103 +196,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -630,7 +534,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,7 +573,7 @@
         <v>100</v>
       </c>
       <c r="D2" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" s="7">
         <v>0</v>
@@ -683,10 +587,10 @@
         <v>60</v>
       </c>
       <c r="C3" s="8">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="D3" s="8">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
@@ -703,7 +607,7 @@
         <v>88</v>
       </c>
       <c r="D4" s="8">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
@@ -720,7 +624,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="8">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E5" s="8">
         <v>0</v>
@@ -737,7 +641,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="8">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E6" s="8">
         <v>0</v>
@@ -754,7 +658,7 @@
         <v>100</v>
       </c>
       <c r="D7" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E7" s="8">
         <v>0</v>
@@ -771,7 +675,7 @@
         <v>90</v>
       </c>
       <c r="D8" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E8" s="8">
         <v>0</v>
@@ -788,7 +692,7 @@
         <v>83</v>
       </c>
       <c r="D9" s="8">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="E9" s="8">
         <v>0</v>
@@ -805,7 +709,7 @@
         <v>82</v>
       </c>
       <c r="D10" s="8">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="E10" s="8">
         <v>0</v>
@@ -822,7 +726,7 @@
         <v>88</v>
       </c>
       <c r="D11" s="8">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="E11" s="8">
         <v>0</v>
@@ -839,7 +743,7 @@
         <v>70</v>
       </c>
       <c r="D12" s="8">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E12" s="8">
         <v>0</v>
@@ -856,7 +760,7 @@
         <v>85</v>
       </c>
       <c r="D13" s="8">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E13" s="8">
         <v>0</v>
@@ -873,7 +777,7 @@
         <v>90</v>
       </c>
       <c r="D14" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E14" s="8">
         <v>0</v>
@@ -892,16 +796,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E13">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="between">
+  <conditionalFormatting sqref="B2:E14">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>0</formula>
       <formula>40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
       <formula>50</formula>
       <formula>70</formula>
     </cfRule>
@@ -918,8 +822,32 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D2:D13">
     <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -942,72 +870,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="between">
-      <formula>80</formula>
-      <formula>100</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="between">
-      <formula>0</formula>
-      <formula>40</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="between">
-      <formula>50</formula>
-      <formula>70</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
-        <cfvo type="num" val="50"/>
-        <cfvo type="num" val="60"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
-      <formula>80</formula>
-      <formula>100</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="between">
-      <formula>0</formula>
-      <formula>40</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="between">
-      <formula>50</formula>
-      <formula>70</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
-        <cfvo type="num" val="50"/>
-        <cfvo type="num" val="60"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
-      <formula>80</formula>
-      <formula>100</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
-      <formula>0</formula>
-      <formula>40</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="between">
-      <formula>50</formula>
-      <formula>70</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E14">
     <cfRule type="colorScale" priority="4">
       <colorScale>
@@ -1020,20 +882,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
-      <formula>80</formula>
-      <formula>100</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
-      <formula>0</formula>
-      <formula>40</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
-      <formula>50</formula>
-      <formula>70</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
agregar interfaz de ver-venta
</commit_message>
<xml_diff>
--- a/Calendario-Responsabilidades.xlsx
+++ b/Calendario-Responsabilidades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\Proyecto-Dorikam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMETH\IdeaProjects\Proyecto-Dorikam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD40FE28-873E-48AB-B09E-CDA458DDB4D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FB41E6-6D8A-4C2B-B7BA-FF2B7DF64571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00253EC3-853E-4A73-9C54-93DBFD01F7E4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00253EC3-853E-4A73-9C54-93DBFD01F7E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,103 +196,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -630,18 +534,18 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="27.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="27.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.88671875" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="29.88671875" customWidth="1"/>
+    <col min="5" max="5" width="30.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="25.15" customHeight="1">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -658,7 +562,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
+    <row r="2" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,13 +573,13 @@
         <v>100</v>
       </c>
       <c r="D2" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
+    <row r="3" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -683,16 +587,16 @@
         <v>60</v>
       </c>
       <c r="C3" s="8">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="D3" s="8">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -703,13 +607,13 @@
         <v>88</v>
       </c>
       <c r="D4" s="8">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -720,13 +624,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="8">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E5" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -737,13 +641,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="8">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E6" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -754,13 +658,13 @@
         <v>100</v>
       </c>
       <c r="D7" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E7" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
+    <row r="8" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -771,13 +675,13 @@
         <v>90</v>
       </c>
       <c r="D8" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E8" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
+    <row r="9" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -788,13 +692,13 @@
         <v>83</v>
       </c>
       <c r="D9" s="8">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="E9" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
+    <row r="10" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -805,13 +709,13 @@
         <v>82</v>
       </c>
       <c r="D10" s="8">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="E10" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" ht="25.15" customHeight="1">
+    <row r="11" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -822,13 +726,13 @@
         <v>88</v>
       </c>
       <c r="D11" s="8">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="E11" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="25.15" customHeight="1">
+    <row r="12" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -839,13 +743,13 @@
         <v>70</v>
       </c>
       <c r="D12" s="8">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E12" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="25.15" customHeight="1">
+    <row r="13" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -856,13 +760,13 @@
         <v>85</v>
       </c>
       <c r="D13" s="8">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E13" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="25.15" customHeight="1">
+    <row r="14" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -873,7 +777,7 @@
         <v>90</v>
       </c>
       <c r="D14" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E14" s="8">
         <v>0</v>
@@ -892,16 +796,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E13">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="between">
+  <conditionalFormatting sqref="B2:E14">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>0</formula>
       <formula>40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
       <formula>50</formula>
       <formula>70</formula>
     </cfRule>
@@ -918,8 +822,32 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D2:D13">
     <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -942,72 +870,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="between">
-      <formula>80</formula>
-      <formula>100</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="between">
-      <formula>0</formula>
-      <formula>40</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="between">
-      <formula>50</formula>
-      <formula>70</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
-        <cfvo type="num" val="50"/>
-        <cfvo type="num" val="60"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
-      <formula>80</formula>
-      <formula>100</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="between">
-      <formula>0</formula>
-      <formula>40</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="between">
-      <formula>50</formula>
-      <formula>70</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
-        <cfvo type="num" val="50"/>
-        <cfvo type="num" val="60"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
-      <formula>80</formula>
-      <formula>100</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
-      <formula>0</formula>
-      <formula>40</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="between">
-      <formula>50</formula>
-      <formula>70</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E14">
     <cfRule type="colorScale" priority="4">
       <colorScale>
@@ -1020,20 +882,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
-      <formula>80</formula>
-      <formula>100</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
-      <formula>0</formula>
-      <formula>40</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
-      <formula>50</formula>
-      <formula>70</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
logica para subir imagenes a la interfaz de ver productos
</commit_message>
<xml_diff>
--- a/Calendario-Responsabilidades.xlsx
+++ b/Calendario-Responsabilidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMETH\IdeaProjects\Proyecto-Dorikam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FB41E6-6D8A-4C2B-B7BA-FF2B7DF64571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F343E8B-8EFF-48A8-83D4-23658C146AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00253EC3-853E-4A73-9C54-93DBFD01F7E4}"/>
   </bookViews>
@@ -534,7 +534,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,7 +576,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -593,7 +593,7 @@
         <v>80</v>
       </c>
       <c r="E3" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -610,7 +610,7 @@
         <v>88</v>
       </c>
       <c r="E4" s="8">
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -627,7 +627,7 @@
         <v>60</v>
       </c>
       <c r="E5" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -644,7 +644,7 @@
         <v>60</v>
       </c>
       <c r="E6" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -661,7 +661,7 @@
         <v>100</v>
       </c>
       <c r="E7" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -678,7 +678,7 @@
         <v>100</v>
       </c>
       <c r="E8" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -695,7 +695,7 @@
         <v>85</v>
       </c>
       <c r="E9" s="8">
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -712,7 +712,7 @@
         <v>85</v>
       </c>
       <c r="E10" s="8">
-        <v>0</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -726,10 +726,10 @@
         <v>88</v>
       </c>
       <c r="D11" s="8">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E11" s="8">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -743,10 +743,10 @@
         <v>70</v>
       </c>
       <c r="D12" s="8">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E12" s="8">
-        <v>0</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -757,13 +757,13 @@
         <v>0</v>
       </c>
       <c r="C13" s="8">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="D13" s="8">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E13" s="8">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -780,7 +780,7 @@
         <v>100</v>
       </c>
       <c r="E14" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
logica para mostrar los productos en TableView y buscar productos
</commit_message>
<xml_diff>
--- a/Calendario-Responsabilidades.xlsx
+++ b/Calendario-Responsabilidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMETH\IdeaProjects\Proyecto-Dorikam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F343E8B-8EFF-48A8-83D4-23658C146AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2A3A1F-7B64-4900-8B1E-29CF6574E567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00253EC3-853E-4A73-9C54-93DBFD01F7E4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>AdministradorController</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>App</t>
+  </si>
+  <si>
+    <t>"01/04/2024" al "07/04/2024"</t>
   </si>
 </sst>
 </file>
@@ -196,7 +199,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -531,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2790D138-02F1-46FC-AFAF-C1A947E3BEF4}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,9 +570,10 @@
     <col min="3" max="3" width="29.6640625" customWidth="1"/>
     <col min="4" max="4" width="29.88671875" customWidth="1"/>
     <col min="5" max="5" width="30.21875" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -561,8 +589,11 @@
       <c r="E1" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,8 +609,11 @@
       <c r="E2" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -595,8 +629,11 @@
       <c r="E3" s="8">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -612,8 +649,11 @@
       <c r="E4" s="8">
         <v>88</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="8">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -629,8 +669,11 @@
       <c r="E5" s="8">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -646,8 +689,11 @@
       <c r="E6" s="8">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -663,8 +709,11 @@
       <c r="E7" s="8">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -680,8 +729,11 @@
       <c r="E8" s="8">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -697,8 +749,11 @@
       <c r="E9" s="8">
         <v>88</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="8">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -714,8 +769,11 @@
       <c r="E10" s="8">
         <v>91</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="8">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -731,8 +789,11 @@
       <c r="E11" s="8">
         <v>90</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -748,8 +809,11 @@
       <c r="E12" s="8">
         <v>70</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -765,8 +829,11 @@
       <c r="E13" s="8">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -782,10 +849,13 @@
       <c r="E14" s="8">
         <v>100</v>
       </c>
+      <c r="F14" s="8">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B14">
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -797,20 +867,44 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
       <formula>0</formula>
       <formula>40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="between">
       <formula>50</formula>
       <formula>70</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C13">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
@@ -822,7 +916,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
+  <conditionalFormatting sqref="D14">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
@@ -834,8 +928,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D13">
-    <cfRule type="colorScale" priority="32">
+  <conditionalFormatting sqref="E2:E13">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -846,7 +940,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
+  <conditionalFormatting sqref="E14:F14">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
@@ -858,19 +952,21 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E13">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
-        <cfvo type="num" val="50"/>
-        <cfvo type="num" val="60"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
+  <conditionalFormatting sqref="F2:F14">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+      <formula>80</formula>
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>0</formula>
+      <formula>40</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
+      <formula>50</formula>
+      <formula>70</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
+  <conditionalFormatting sqref="F2:F13">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>

</xml_diff>

<commit_message>
Calendario (Interfaz Reportes 100%)
</commit_message>
<xml_diff>
--- a/Calendario-Responsabilidades.xlsx
+++ b/Calendario-Responsabilidades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMETH\IdeaProjects\Proyecto-Dorikam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rumba Hospitality\Documents\ProyectosJavaFX\Proyecto-Dorikam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2A3A1F-7B64-4900-8B1E-29CF6574E567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70EB9B6-7B62-4D0C-87D6-2E948F582A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00253EC3-853E-4A73-9C54-93DBFD01F7E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00253EC3-853E-4A73-9C54-93DBFD01F7E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,31 +199,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -262,9 +238,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -302,7 +278,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -408,7 +384,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -550,7 +526,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -561,19 +537,19 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="27.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="27.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.88671875" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" customWidth="1"/>
-    <col min="4" max="4" width="29.88671875" customWidth="1"/>
-    <col min="5" max="5" width="30.21875" customWidth="1"/>
-    <col min="6" max="6" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="25.15" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -593,7 +569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -613,7 +589,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -633,7 +609,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -653,7 +629,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -673,7 +649,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -693,7 +669,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -713,7 +689,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -733,7 +709,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -753,7 +729,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -773,7 +749,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" s="3" customFormat="1" ht="25.15" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -793,7 +769,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="25.15" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -813,7 +789,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="25.15" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -827,13 +803,13 @@
         <v>60</v>
       </c>
       <c r="E13" s="8">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="F13" s="8">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="25.15" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -866,16 +842,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
+  <conditionalFormatting sqref="B2:F14">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>0</formula>
       <formula>40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
       <formula>50</formula>
       <formula>70</formula>
     </cfRule>
@@ -952,20 +928,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F14">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
-      <formula>80</formula>
-      <formula>100</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
-      <formula>0</formula>
-      <formula>40</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
-      <formula>50</formula>
-      <formula>70</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F2:F13">
     <cfRule type="colorScale" priority="4">
       <colorScale>

</xml_diff>

<commit_message>
Logica para apartar productos
</commit_message>
<xml_diff>
--- a/Calendario-Responsabilidades.xlsx
+++ b/Calendario-Responsabilidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMETH\IdeaProjects\Proyecto-Dorikam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2A3A1F-7B64-4900-8B1E-29CF6574E567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2CA2CF-5DD5-4249-9F52-EE4F11E3CE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00253EC3-853E-4A73-9C54-93DBFD01F7E4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>AdministradorController</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>"01/04/2024" al "07/04/2024"</t>
+  </si>
+  <si>
+    <t>Aplicar Herencia</t>
   </si>
 </sst>
 </file>
@@ -199,31 +202,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -558,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2790D138-02F1-46FC-AFAF-C1A947E3BEF4}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -830,7 +809,7 @@
         <v>60</v>
       </c>
       <c r="F13" s="8">
-        <v>60</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -853,9 +832,29 @@
         <v>100</v>
       </c>
     </row>
+    <row r="15" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B14">
-    <cfRule type="colorScale" priority="45">
+  <conditionalFormatting sqref="B2:B15">
+    <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -866,21 +865,45 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
+  <conditionalFormatting sqref="B2:F15">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>0</formula>
       <formula>40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
       <formula>50</formula>
       <formula>70</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C13">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:C15">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
@@ -892,7 +915,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
+  <conditionalFormatting sqref="D14:D15">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
@@ -904,8 +927,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D13">
-    <cfRule type="colorScale" priority="36">
+  <conditionalFormatting sqref="E2:E13">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -916,7 +939,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
+  <conditionalFormatting sqref="E14:F14">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
@@ -928,8 +951,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E13">
-    <cfRule type="colorScale" priority="23">
+  <conditionalFormatting sqref="E15:F15">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -940,7 +963,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14:F14">
+  <conditionalFormatting sqref="F2:F13">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
@@ -952,32 +975,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F14">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
-      <formula>80</formula>
-      <formula>100</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
-      <formula>0</formula>
-      <formula>40</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
-      <formula>50</formula>
-      <formula>70</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F13">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
-        <cfvo type="num" val="50"/>
-        <cfvo type="num" val="60"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Implementacion localDate y LocalTime en el Home
</commit_message>
<xml_diff>
--- a/Calendario-Responsabilidades.xlsx
+++ b/Calendario-Responsabilidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMETH\IdeaProjects\Proyecto-Dorikam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53266452-C2B9-4CE8-A377-AA0A4EF27EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6578FB03-D407-49B7-A7E8-0EF589B92193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00253EC3-853E-4A73-9C54-93DBFD01F7E4}"/>
   </bookViews>
@@ -540,7 +540,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -729,7 +729,7 @@
         <v>88</v>
       </c>
       <c r="F9" s="8">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -749,7 +749,7 @@
         <v>91</v>
       </c>
       <c r="F10" s="8">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Logica para subir imagenes al catalogo desde la interfaz de AgregarProductos
</commit_message>
<xml_diff>
--- a/Calendario-Responsabilidades.xlsx
+++ b/Calendario-Responsabilidades.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMETH\IdeaProjects\Proyecto-Dorikam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6578FB03-D407-49B7-A7E8-0EF589B92193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BD99D0-1E33-4D28-8A51-0B03164110E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00253EC3-853E-4A73-9C54-93DBFD01F7E4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>AdministradorController</t>
   </si>
@@ -85,13 +85,16 @@
   </si>
   <si>
     <t>Aplicar Herencia</t>
+  </si>
+  <si>
+    <t>Detalles de FrontEnd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,8 +127,15 @@
       <family val="2"/>
       <charset val="128"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Coolvetica Rg"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +151,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -172,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -198,11 +214,36 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -537,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2790D138-02F1-46FC-AFAF-C1A947E3BEF4}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -852,9 +893,29 @@
         <v>100</v>
       </c>
     </row>
+    <row r="17" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="8">
+        <v>20</v>
+      </c>
+      <c r="C17" s="8">
+        <v>50</v>
+      </c>
+      <c r="D17" s="8">
+        <v>55</v>
+      </c>
+      <c r="E17" s="8">
+        <v>80</v>
+      </c>
+      <c r="F17" s="8">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B15">
-    <cfRule type="colorScale" priority="49">
+    <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>
@@ -866,6 +927,128 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F15">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="between">
+      <formula>80</formula>
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="between">
+      <formula>0</formula>
+      <formula>40</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="between">
+      <formula>50</formula>
+      <formula>70</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C13">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:C15">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D13">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14:D15">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E13">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:F14">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15:F15">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F13">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:F17">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>80</formula>
       <formula>100</formula>
@@ -879,92 +1062,32 @@
       <formula>70</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C13">
-    <cfRule type="colorScale" priority="44">
-      <colorScale>
-        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
-        <cfvo type="num" val="50"/>
-        <cfvo type="num" val="60"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14:C15">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
-        <cfvo type="num" val="50"/>
-        <cfvo type="num" val="60"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D13">
-    <cfRule type="colorScale" priority="40">
-      <colorScale>
-        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
-        <cfvo type="num" val="50"/>
-        <cfvo type="num" val="60"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D15">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
-        <cfvo type="num" val="50"/>
-        <cfvo type="num" val="60"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E13">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
-        <cfvo type="num" val="50"/>
-        <cfvo type="num" val="60"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:F14">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
-        <cfvo type="num" val="50"/>
-        <cfvo type="num" val="60"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15:F15">
+  <conditionalFormatting sqref="C17">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:F17">
     <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
-        <cfvo type="num" val="50"/>
-        <cfvo type="num" val="60"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F13">
-    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="percent" val="&quot;10% a 40%&quot;"/>
         <cfvo type="num" val="50"/>

</xml_diff>